<commit_message>
fix: Error no view subscription item
</commit_message>
<xml_diff>
--- a/public/files/sample_file.xlsx
+++ b/public/files/sample_file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\CGV_Telecom_Booking_V1_Front-End\public\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FAD37F2-28FE-421A-BF26-4547BE74A300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD18DCE-33C9-4EE4-AD0A-64E8872A6C0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{F038391C-AC66-43F7-8E29-578F14832AAD}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="17">
   <si>
     <t>Số điện thoại</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>0919098898</t>
+  </si>
+  <si>
+    <t>Tên khách hàng</t>
   </si>
 </sst>
 </file>
@@ -462,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8126F7F4-9726-480C-98F2-5877011EB363}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -475,9 +478,10 @@
     <col min="4" max="4" width="10.1328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.1328125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -499,8 +503,11 @@
       <c r="G1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -520,7 +527,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -540,7 +547,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -560,7 +567,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -580,7 +587,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -600,7 +607,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>

</xml_diff>